<commit_message>
rename delay to latency and uncomment anova
</commit_message>
<xml_diff>
--- a/Stats/delays_by_platforms.xlsx
+++ b/Stats/delays_by_platforms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoltan.tudlik/AaltoDevelopment/ServerlessAtTheEdgeMeasurements/Stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4219E159-719F-8242-BB7E-2E93E9F42C17}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CC315E-E0F1-8249-97C5-77F946464DDF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,9 +33,6 @@
     <t xml:space="preserve">Measure:   MEASURE_1  </t>
   </si>
   <si>
-    <t>delayType</t>
-  </si>
-  <si>
     <t>Mean</t>
   </si>
   <si>
@@ -72,16 +69,19 @@
     <t>,101</t>
   </si>
   <si>
-    <t>Network delay</t>
-  </si>
-  <si>
-    <t>Processing delay</t>
-  </si>
-  <si>
     <t>AWS Greengrass</t>
   </si>
   <si>
     <t>AWS IoT</t>
+  </si>
+  <si>
+    <t>latencyType</t>
+  </si>
+  <si>
+    <t>Network latency</t>
+  </si>
+  <si>
+    <t>Processing latency</t>
   </si>
 </sst>
 </file>
@@ -506,10 +506,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Network delay</c:v>
+                  <c:v>Network latency</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Processing delay</c:v>
+                  <c:v>Processing latency</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -591,10 +591,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Network delay</c:v>
+                  <c:v>Network latency</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Processing delay</c:v>
+                  <c:v>Processing latency</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -668,7 +668,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="hu-HU"/>
-                  <a:t>Delay mean</a:t>
+                  <a:t>Latency mean</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="hu-HU" baseline="0"/>
@@ -1074,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="190" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="190" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1105,16 +1105,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="D3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="E3" s="25" t="s">
         <v>5</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>6</v>
       </c>
       <c r="F3" s="26"/>
     </row>
@@ -1124,18 +1124,18 @@
       <c r="C4" s="22"/>
       <c r="D4" s="24"/>
       <c r="E4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="C5" s="1">
         <v>9.5000000000000001E-2</v>
@@ -1144,18 +1144,18 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="41" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C6" s="9">
         <v>0.375</v>
@@ -1164,15 +1164,15 @@
         <v>1E-3</v>
       </c>
       <c r="E6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>11</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7" s="11">
         <v>1</v>
@@ -1184,15 +1184,15 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B8" s="12">
         <v>2</v>
@@ -1204,10 +1204,10 @@
         <v>1E-3</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>

</xml_diff>